<commit_message>
modified for server's data
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/GameServer.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/GameServer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>ServerID</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameServer_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000104001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,7 +465,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="A2:I7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -489,8 +501,27 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>4001</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1"/>
@@ -515,7 +546,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>